<commit_message>
Began brainstorming file encryption strategy. Published BlazorPWA.
</commit_message>
<xml_diff>
--- a/SafeSecrets Design Notes.xlsx
+++ b/SafeSecrets Design Notes.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glenw\Dropbox\Personal\Hobbies\Software Dev Projects\JavaScript Projects\SafeSecrets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A6A1AE-B264-4951-A4DB-F828814C619A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5772A368-2CF8-4AB9-A98F-BD20929CE006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="300" windowWidth="29295" windowHeight="20295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2085" yWindow="2775" windowWidth="18390" windowHeight="18030" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UI Design" sheetId="1" r:id="rId1"/>
-    <sheet name="Performance" sheetId="2" r:id="rId2"/>
-    <sheet name="Common File Extensions" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
+    <sheet name="File Decryption Sequence" sheetId="3" r:id="rId2"/>
+    <sheet name="Performance" sheetId="2" r:id="rId3"/>
+    <sheet name="Common File Extensions" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="2" hidden="1">'Common File Extensions'!$A$1:$B$179</definedName>
+    <definedName name="ExternalData_1" localSheetId="3" hidden="1">'Common File Extensions'!$A$1:$B$179</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="354">
   <si>
     <t>SafeSecrets</t>
   </si>
@@ -1125,6 +1125,24 @@
   </si>
   <si>
     <t>Microsoft Excel 97 document. Can contain malicious macro code.</t>
+  </si>
+  <si>
+    <t>CONTENT: JSON with software version number, PIN hint, encrypted data.</t>
+  </si>
+  <si>
+    <t>CONTENT: All file data. File content was encrypted to give no clues about software used for decryption.</t>
+  </si>
+  <si>
+    <t>DECRYPT WITH:</t>
+  </si>
+  <si>
+    <t>CONTENT:</t>
+  </si>
+  <si>
+    <t>DECRYPT WITH: RAS, key=PBDGKF2(&lt;PIN&gt;+&lt;stored software version number&gt;)+&lt;small random salt selected from [reduced set of 2-byte UTF-8 as defined by PIN]?&gt;</t>
+  </si>
+  <si>
+    <t>DECRYPT WITH: AES, key=SHA256("SafeSecrets"+&lt;some standard hardcoded salt&gt;)+&lt;small random salt&gt;</t>
   </si>
 </sst>
 </file>
@@ -1348,7 +1366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1359,15 +1377,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1388,15 +1397,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1416,24 +1432,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
         <vertical style="thin">
           <color indexed="64"/>
         </vertical>
@@ -1492,6 +1490,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -1506,12 +1520,14 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
+        <top/>
+        <bottom/>
+        <vertical style="thin">
           <color indexed="64"/>
-        </top>
-        <bottom style="thin">
+        </vertical>
+        <horizontal style="thin">
           <color indexed="64"/>
-        </bottom>
+        </horizontal>
       </border>
     </dxf>
   </dxfs>
@@ -1528,23 +1544,23 @@
 </file>
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{978C9E23-D4B0-11CE-BF2D-00AA003F40D0}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX10.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX11.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{978C9E23-D4B0-11CE-BF2D-00AA003F40D0}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX12.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
-<file path=xl/activeX/activeX10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX13.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{978C9E23-D4B0-11CE-BF2D-00AA003F40D0}" ax:persistence="persistStreamInit" r:id="rId1"/>
-</file>
-
-<file path=xl/activeX/activeX11.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
-</file>
-
-<file path=xl/activeX/activeX12.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
-</file>
-
-<file path=xl/activeX/activeX13.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX14.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1552,7 +1568,7 @@
 </file>
 
 <file path=xl/activeX/activeX15.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{978C9E23-D4B0-11CE-BF2D-00AA003F40D0}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1560,23 +1576,23 @@
 </file>
 
 <file path=xl/activeX/activeX3.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX6.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{978C9E23-D4B0-11CE-BF2D-00AA003F40D0}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
-<file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX7.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
-</file>
-
-<file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{978C9E23-D4B0-11CE-BF2D-00AA003F40D0}" ax:persistence="persistStreamInit" r:id="rId1"/>
-</file>
-
-<file path=xl/activeX/activeX6.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
-</file>
-
-<file path=xl/activeX/activeX7.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1584,7 +1600,7 @@
 </file>
 
 <file path=xl/activeX/activeX9.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2475,14 +2491,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5C44BE27-0A17-4F23-A900-DA272980895F}" name="Common_File_Extensions" displayName="Common_File_Extensions" ref="A1:C179" tableType="queryTable" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5C44BE27-0A17-4F23-A900-DA272980895F}" name="Common_File_Extensions" displayName="Common_File_Extensions" ref="A1:C179" tableType="queryTable" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A1:C179" xr:uid="{5C44BE27-0A17-4F23-A900-DA272980895F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C179">
     <sortCondition ref="A1:A179"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{20F0EF45-D9DD-4951-B0E0-C56102E13C80}" uniqueName="1" name="Extension" queryTableFieldId="1" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{CFCDB360-6C0D-4B8B-9B43-78275C051250}" uniqueName="2" name="Description" queryTableFieldId="2" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{20F0EF45-D9DD-4951-B0E0-C56102E13C80}" uniqueName="1" name="Extension" queryTableFieldId="1" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{CFCDB360-6C0D-4B8B-9B43-78275C051250}" uniqueName="2" name="Description" queryTableFieldId="2" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{33C7DA5A-E0CB-4123-9BCF-95929110E1DE}" uniqueName="3" name="Is Restricted" queryTableFieldId="3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2767,24 +2783,24 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3148,40 +3164,40 @@
       <c r="H38" s="7"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="24"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="25"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="24"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3195,143 +3211,68 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1037" r:id="rId3" name="TextBox4">
+        <control shapeId="1039" r:id="rId3" name="Label6">
           <controlPr defaultSize="0" autoLine="0" r:id="rId4">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>571500</xdr:colOff>
-                <xdr:row>25</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>485775</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>7</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1037" r:id="rId3" name="TextBox4"/>
+        <control shapeId="1039" r:id="rId3" name="Label6"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1036" r:id="rId5" name="Label4">
+        <control shapeId="1038" r:id="rId5" name="Label5">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>25</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>381000</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>552450</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>152400</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1036" r:id="rId5" name="Label4"/>
+        <control shapeId="1038" r:id="rId5" name="Label5"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1035" r:id="rId7" name="Label3">
+        <control shapeId="1025" r:id="rId7" name="CommandButton1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId8">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>552450</xdr:colOff>
-                <xdr:row>25</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1035" r:id="rId7" name="Label3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1034" r:id="rId9" name="TextBox3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>571500</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>495300</xdr:colOff>
+                <xdr:row>35</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>7</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>25</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1034" r:id="rId9" name="TextBox3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1033" r:id="rId11" name="Label2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>35</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1033" r:id="rId11" name="Label2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1032" r:id="rId13" name="CommandButton5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>342900</xdr:colOff>
-                <xdr:row>35</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>37</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </to>
@@ -3340,23 +3281,23 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1032" r:id="rId13" name="CommandButton5"/>
+        <control shapeId="1025" r:id="rId7" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1031" r:id="rId15" name="CommandButton4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
+        <control shapeId="1026" r:id="rId9" name="CommandButton2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>152400</xdr:colOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>76200</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>323850</xdr:colOff>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>123825</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>161925</xdr:rowOff>
               </to>
@@ -3365,7 +3306,82 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1031" r:id="rId15" name="CommandButton4"/>
+        <control shapeId="1026" r:id="rId9" name="CommandButton2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1027" r:id="rId11" name="TextBox1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1027" r:id="rId11" name="TextBox1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1028" r:id="rId13" name="Label1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>123825</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1028" r:id="rId13" name="Label1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1029" r:id="rId15" name="TextBox2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>142875</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1029" r:id="rId15" name="TextBox2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3395,93 +3411,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1029" r:id="rId19" name="TextBox2">
+        <control shapeId="1031" r:id="rId19" name="CommandButton4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId20">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>2</xdr:col>
-                <xdr:colOff>142875</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1029" r:id="rId19" name="TextBox2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId21" name="Label1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>123825</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1028" r:id="rId21" name="Label1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId23" name="TextBox1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId24">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1027" r:id="rId23" name="TextBox1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId25" name="CommandButton2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId26">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:colOff>152400</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>76200</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>123825</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>323850</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>161925</xdr:rowOff>
               </to>
@@ -3490,23 +3431,23 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId25" name="CommandButton2"/>
+        <control shapeId="1031" r:id="rId19" name="CommandButton4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId27" name="CommandButton1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId28">
+        <control shapeId="1032" r:id="rId21" name="CommandButton5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>495300</xdr:colOff>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>342900</xdr:colOff>
                 <xdr:row>35</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>37</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </to>
@@ -3515,57 +3456,132 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId27" name="CommandButton1"/>
+        <control shapeId="1032" r:id="rId21" name="CommandButton5"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1038" r:id="rId29" name="Label5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId30">
+        <control shapeId="1033" r:id="rId23" name="Label2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId24">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>381000</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>152400</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>35</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1038" r:id="rId29" name="Label5"/>
+        <control shapeId="1033" r:id="rId23" name="Label2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1039" r:id="rId31" name="Label6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId32">
+        <control shapeId="1034" r:id="rId25" name="TextBox3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId26">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>485775</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>571500</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>7</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1039" r:id="rId31" name="Label6"/>
+        <control shapeId="1034" r:id="rId25" name="TextBox3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1035" r:id="rId27" name="Label3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId28">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>552450</xdr:colOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1035" r:id="rId27" name="Label3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1036" r:id="rId29" name="Label4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId30">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>552450</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1036" r:id="rId29" name="Label4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1037" r:id="rId31" name="TextBox4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId32">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>571500</xdr:colOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1037" r:id="rId31" name="TextBox4"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3573,6 +3589,591 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80036CEE-20A2-4D5B-894A-BFFA26FC4F58}">
+  <dimension ref="A1:D42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97CE5E0-6055-418C-B30C-96F3C1ED1011}">
   <dimension ref="A1:E21"/>
   <sheetViews>
@@ -3582,2234 +4183,2233 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="78.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="11">
         <f>10111/55</f>
         <v>183.83636363636364</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
+      <c r="A3" s="9">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="11">
         <f>10111/55</f>
         <v>183.83636363636364</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
+      <c r="A4" s="9">
         <v>1</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="11">
         <f>10111/54</f>
         <v>187.24074074074073</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
+      <c r="A5" s="9">
         <v>1</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="11">
         <f>10111/54</f>
         <v>187.24074074074073</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="A6" s="9">
         <v>1</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="11">
         <f>10111/57</f>
         <v>177.38596491228071</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
+      <c r="A7" s="9">
         <v>1</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="11">
         <f>10111/49</f>
         <v>206.34693877551021</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+      <c r="A8" s="9">
         <v>1</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="11">
         <f>10111/104</f>
         <v>97.22115384615384</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="13"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="13"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="13"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="10"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="13"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="13"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="10"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="13"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="13"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="13"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="10"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="13"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="10"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="13"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="13"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="10"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="13"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="10"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="13"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E6D3D21-9B6A-4A58-AF92-18A0BE64C7A5}">
   <dimension ref="A1:C179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A127" workbookViewId="0">
       <selection activeCell="A175" sqref="A175:XFD175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="19" customWidth="1"/>
-    <col min="2" max="2" width="74.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="19"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="74.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="16" t="s">
         <v>275</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="17" t="s">
         <v>276</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="19" t="s">
         <v>230</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="18" t="s">
         <v>283</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="19" t="s">
         <v>284</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="18" t="s">
         <v>293</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="19" t="s">
         <v>294</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="18" t="s">
         <v>208</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="18" t="s">
         <v>295</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="19" t="s">
         <v>294</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="19" t="s">
         <v>211</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="18" t="s">
         <v>183</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="23" t="s">
+      <c r="A32" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="19" t="s">
         <v>213</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="23" t="s">
+      <c r="A33" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="24" t="s">
+      <c r="B33" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="24" t="s">
+      <c r="B34" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="23" t="s">
+      <c r="A35" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B35" s="24" t="s">
+      <c r="B35" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="24" t="s">
+      <c r="B36" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="18" t="s">
         <v>214</v>
       </c>
-      <c r="B37" s="24" t="s">
+      <c r="B37" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="23" t="s">
+      <c r="A38" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="24" t="s">
+      <c r="B38" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="23" t="s">
+      <c r="A39" s="18" t="s">
         <v>216</v>
       </c>
-      <c r="B39" s="24" t="s">
+      <c r="B39" s="19" t="s">
         <v>217</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="23" t="s">
+      <c r="A40" s="18" t="s">
         <v>260</v>
       </c>
-      <c r="B40" s="24" t="s">
+      <c r="B40" s="19" t="s">
         <v>343</v>
       </c>
-      <c r="C40" s="20" t="s">
+      <c r="C40" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="23" t="s">
+      <c r="A41" s="18" t="s">
         <v>333</v>
       </c>
-      <c r="B41" s="24" t="s">
+      <c r="B41" s="19" t="s">
         <v>334</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C41" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="18" t="s">
         <v>261</v>
       </c>
-      <c r="B42" s="24" t="s">
+      <c r="B42" s="19" t="s">
         <v>262</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="C42" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="23" t="s">
+      <c r="A43" s="18" t="s">
         <v>335</v>
       </c>
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="19" t="s">
         <v>334</v>
       </c>
-      <c r="C43" s="20" t="s">
+      <c r="C43" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="23" t="s">
+      <c r="A44" s="18" t="s">
         <v>218</v>
       </c>
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C44" s="13" t="s">
+      <c r="C44" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="B45" s="24" t="s">
+      <c r="B45" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="C45" s="13" t="s">
+      <c r="C45" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="23" t="s">
+      <c r="A46" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="B46" s="24" t="s">
+      <c r="B46" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="C46" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="23" t="s">
+      <c r="A47" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="B47" s="24" t="s">
+      <c r="B47" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="C47" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="23" t="s">
+      <c r="A48" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="B48" s="24" t="s">
+      <c r="B48" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="C48" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="23" t="s">
+      <c r="A49" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="B49" s="24" t="s">
+      <c r="B49" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="C49" s="13" t="s">
+      <c r="C49" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="23" t="s">
+      <c r="A50" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="B50" s="24" t="s">
+      <c r="B50" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="C50" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="23" t="s">
+      <c r="A51" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="B51" s="24" t="s">
+      <c r="B51" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="C51" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="23" t="s">
+      <c r="A52" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="24" t="s">
+      <c r="B52" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="C52" s="13" t="s">
+      <c r="C52" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="23" t="s">
+      <c r="A53" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="B53" s="24" t="s">
+      <c r="B53" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="C53" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="23" t="s">
+      <c r="A54" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B54" s="24" t="s">
+      <c r="B54" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C54" s="13" t="s">
+      <c r="C54" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="23" t="s">
+      <c r="A55" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="B55" s="24" t="s">
+      <c r="B55" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="C55" s="13" t="s">
+      <c r="C55" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="23" t="s">
+      <c r="A56" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="B56" s="24" t="s">
+      <c r="B56" s="19" t="s">
         <v>238</v>
       </c>
-      <c r="C56" s="13" t="s">
+      <c r="C56" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="23" t="s">
+      <c r="A57" s="18" t="s">
         <v>289</v>
       </c>
-      <c r="B57" s="24" t="s">
+      <c r="B57" s="19" t="s">
         <v>290</v>
       </c>
-      <c r="C57" s="20" t="s">
+      <c r="C57" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="23" t="s">
+      <c r="A58" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="B58" s="24" t="s">
+      <c r="B58" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="C58" s="13" t="s">
+      <c r="C58" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="23" t="s">
+      <c r="A59" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="B59" s="24" t="s">
+      <c r="B59" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="C59" s="13" t="s">
+      <c r="C59" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="23" t="s">
+      <c r="A60" s="18" t="s">
         <v>220</v>
       </c>
-      <c r="B60" s="24" t="s">
+      <c r="B60" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="C60" s="13" t="s">
+      <c r="C60" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="23" t="s">
+      <c r="A61" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="B61" s="24" t="s">
+      <c r="B61" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="C61" s="13" t="s">
+      <c r="C61" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="23" t="s">
+      <c r="A62" s="18" t="s">
         <v>327</v>
       </c>
-      <c r="B62" s="24" t="s">
+      <c r="B62" s="19" t="s">
         <v>328</v>
       </c>
-      <c r="C62" s="20" t="s">
+      <c r="C62" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="23" t="s">
+      <c r="A63" s="18" t="s">
         <v>222</v>
       </c>
-      <c r="B63" s="24" t="s">
+      <c r="B63" s="19" t="s">
         <v>223</v>
       </c>
-      <c r="C63" s="13" t="s">
+      <c r="C63" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="23" t="s">
+      <c r="A64" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="B64" s="24" t="s">
+      <c r="B64" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="C64" s="13" t="s">
+      <c r="C64" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="23" t="s">
+      <c r="A65" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="B65" s="24" t="s">
+      <c r="B65" s="19" t="s">
         <v>344</v>
       </c>
-      <c r="C65" s="13" t="s">
+      <c r="C65" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="23" t="s">
+      <c r="A66" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="B66" s="24" t="s">
+      <c r="B66" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="C66" s="13" t="s">
+      <c r="C66" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="23" t="s">
+      <c r="A67" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="B67" s="24" t="s">
+      <c r="B67" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="C67" s="13" t="s">
+      <c r="C67" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="23" t="s">
+      <c r="A68" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="B68" s="24" t="s">
+      <c r="B68" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="C68" s="13" t="s">
+      <c r="C68" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="23" t="s">
+      <c r="A69" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="B69" s="24" t="s">
+      <c r="B69" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="C69" s="13" t="s">
+      <c r="C69" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="23" t="s">
+      <c r="A70" s="18" t="s">
         <v>301</v>
       </c>
-      <c r="B70" s="24" t="s">
+      <c r="B70" s="19" t="s">
         <v>302</v>
       </c>
-      <c r="C70" s="20" t="s">
+      <c r="C70" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="23" t="s">
+      <c r="A71" s="18" t="s">
         <v>303</v>
       </c>
-      <c r="B71" s="24" t="s">
+      <c r="B71" s="19" t="s">
         <v>304</v>
       </c>
-      <c r="C71" s="20" t="s">
+      <c r="C71" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="23" t="s">
+      <c r="A72" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="B72" s="24" t="s">
+      <c r="B72" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="C72" s="13" t="s">
+      <c r="C72" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="23" t="s">
+      <c r="A73" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="B73" s="24" t="s">
+      <c r="B73" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="C73" s="13" t="s">
+      <c r="C73" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="23" t="s">
+      <c r="A74" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="B74" s="24" t="s">
+      <c r="B74" s="19" t="s">
         <v>345</v>
       </c>
-      <c r="C74" s="13" t="s">
+      <c r="C74" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="23" t="s">
+      <c r="A75" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B75" s="24" t="s">
+      <c r="B75" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="C75" s="13" t="s">
+      <c r="C75" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="23" t="s">
+      <c r="A76" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="B76" s="24" t="s">
+      <c r="B76" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="C76" s="13" t="s">
+      <c r="C76" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="23" t="s">
+      <c r="A77" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="B77" s="24" t="s">
+      <c r="B77" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="C77" s="13" t="s">
+      <c r="C77" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="23" t="s">
+      <c r="A78" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B78" s="24" t="s">
+      <c r="B78" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C78" s="13" t="s">
+      <c r="C78" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="23" t="s">
+      <c r="A79" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B79" s="24" t="s">
+      <c r="B79" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C79" s="13" t="s">
+      <c r="C79" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="23" t="s">
+      <c r="A80" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="B80" s="24" t="s">
+      <c r="B80" s="19" t="s">
         <v>242</v>
       </c>
-      <c r="C80" s="13" t="s">
+      <c r="C80" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="23" t="s">
+      <c r="A81" s="18" t="s">
         <v>243</v>
       </c>
-      <c r="B81" s="24" t="s">
+      <c r="B81" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="C81" s="13" t="s">
+      <c r="C81" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="23" t="s">
+      <c r="A82" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B82" s="24" t="s">
+      <c r="B82" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C82" s="13" t="s">
+      <c r="C82" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="23" t="s">
+      <c r="A83" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="B83" s="24" t="s">
+      <c r="B83" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="C83" s="13" t="s">
+      <c r="C83" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="23" t="s">
+      <c r="A84" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B84" s="24" t="s">
+      <c r="B84" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C84" s="13" t="s">
+      <c r="C84" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="23" t="s">
+      <c r="A85" s="18" t="s">
         <v>249</v>
       </c>
-      <c r="B85" s="24" t="s">
+      <c r="B85" s="19" t="s">
         <v>248</v>
       </c>
-      <c r="C85" s="13" t="s">
+      <c r="C85" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="23" t="s">
+      <c r="A86" s="18" t="s">
         <v>247</v>
       </c>
-      <c r="B86" s="24" t="s">
+      <c r="B86" s="19" t="s">
         <v>248</v>
       </c>
-      <c r="C86" s="13" t="s">
+      <c r="C86" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="23" t="s">
+      <c r="A87" s="18" t="s">
         <v>291</v>
       </c>
-      <c r="B87" s="24" t="s">
+      <c r="B87" s="19" t="s">
         <v>292</v>
       </c>
-      <c r="C87" s="20" t="s">
+      <c r="C87" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="23" t="s">
+      <c r="A88" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="B88" s="24" t="s">
+      <c r="B88" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="C88" s="13" t="s">
+      <c r="C88" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="23" t="s">
+      <c r="A89" s="18" t="s">
         <v>318</v>
       </c>
-      <c r="B89" s="24" t="s">
+      <c r="B89" s="19" t="s">
         <v>319</v>
       </c>
-      <c r="C89" s="20" t="s">
+      <c r="C89" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="23" t="s">
+      <c r="A90" s="18" t="s">
         <v>320</v>
       </c>
-      <c r="B90" s="24" t="s">
+      <c r="B90" s="19" t="s">
         <v>319</v>
       </c>
-      <c r="C90" s="20" t="s">
+      <c r="C90" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="23" t="s">
+      <c r="A91" s="18" t="s">
         <v>323</v>
       </c>
-      <c r="B91" s="24" t="s">
+      <c r="B91" s="19" t="s">
         <v>319</v>
       </c>
-      <c r="C91" s="20" t="s">
+      <c r="C91" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="23" t="s">
+      <c r="A92" s="18" t="s">
         <v>321</v>
       </c>
-      <c r="B92" s="24" t="s">
+      <c r="B92" s="19" t="s">
         <v>319</v>
       </c>
-      <c r="C92" s="20" t="s">
+      <c r="C92" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="23" t="s">
+      <c r="A93" s="18" t="s">
         <v>324</v>
       </c>
-      <c r="B93" s="24" t="s">
+      <c r="B93" s="19" t="s">
         <v>319</v>
       </c>
-      <c r="C93" s="20" t="s">
+      <c r="C93" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="23" t="s">
+      <c r="A94" s="18" t="s">
         <v>322</v>
       </c>
-      <c r="B94" s="24" t="s">
+      <c r="B94" s="19" t="s">
         <v>319</v>
       </c>
-      <c r="C94" s="20" t="s">
+      <c r="C94" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="23" t="s">
+      <c r="A95" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="B95" s="24" t="s">
+      <c r="B95" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="C95" s="13" t="s">
+      <c r="C95" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="23" t="s">
+      <c r="A96" s="18" t="s">
         <v>285</v>
       </c>
-      <c r="B96" s="24" t="s">
+      <c r="B96" s="19" t="s">
         <v>286</v>
       </c>
-      <c r="C96" s="20" t="s">
+      <c r="C96" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="23" t="s">
+      <c r="A97" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="B97" s="24" t="s">
+      <c r="B97" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="C97" s="13" t="s">
+      <c r="C97" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="23" t="s">
+      <c r="A98" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="B98" s="24" t="s">
+      <c r="B98" s="19" t="s">
         <v>199</v>
       </c>
-      <c r="C98" s="13" t="s">
+      <c r="C98" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="23" t="s">
+      <c r="A99" s="18" t="s">
         <v>263</v>
       </c>
-      <c r="B99" s="24" t="s">
+      <c r="B99" s="19" t="s">
         <v>264</v>
       </c>
-      <c r="C99" s="13" t="s">
+      <c r="C99" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="23" t="s">
+      <c r="A100" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="B100" s="24" t="s">
+      <c r="B100" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="C100" s="13" t="s">
+      <c r="C100" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="23" t="s">
+      <c r="A101" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B101" s="24" t="s">
+      <c r="B101" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C101" s="13" t="s">
+      <c r="C101" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="23" t="s">
+      <c r="A102" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="B102" s="24" t="s">
+      <c r="B102" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="C102" s="13" t="s">
+      <c r="C102" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="23" t="s">
+      <c r="A103" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="B103" s="24" t="s">
+      <c r="B103" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="C103" s="13" t="s">
+      <c r="C103" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="23" t="s">
+      <c r="A104" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="B104" s="24" t="s">
+      <c r="B104" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="C104" s="13" t="s">
+      <c r="C104" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="23" t="s">
+      <c r="A105" s="18" t="s">
         <v>265</v>
       </c>
-      <c r="B105" s="24" t="s">
+      <c r="B105" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="C105" s="13" t="s">
+      <c r="C105" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="23" t="s">
+      <c r="A106" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="B106" s="24" t="s">
+      <c r="B106" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="C106" s="13" t="s">
+      <c r="C106" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="23" t="s">
+      <c r="A107" s="18" t="s">
         <v>281</v>
       </c>
-      <c r="B107" s="24" t="s">
+      <c r="B107" s="19" t="s">
         <v>282</v>
       </c>
-      <c r="C107" s="20" t="s">
+      <c r="C107" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="23" t="s">
+      <c r="A108" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B108" s="24" t="s">
+      <c r="B108" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C108" s="13" t="s">
+      <c r="C108" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="23" t="s">
+      <c r="A109" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="B109" s="24" t="s">
+      <c r="B109" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="C109" s="13" t="s">
+      <c r="C109" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="23" t="s">
+      <c r="A110" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="B110" s="24" t="s">
+      <c r="B110" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="C110" s="13" t="s">
+      <c r="C110" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="23" t="s">
+      <c r="A111" s="18" t="s">
         <v>339</v>
       </c>
-      <c r="B111" s="24" t="s">
+      <c r="B111" s="19" t="s">
         <v>334</v>
       </c>
-      <c r="C111" s="20" t="s">
+      <c r="C111" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="23" t="s">
+      <c r="A112" s="18" t="s">
         <v>340</v>
       </c>
-      <c r="B112" s="24" t="s">
+      <c r="B112" s="19" t="s">
         <v>334</v>
       </c>
-      <c r="C112" s="20" t="s">
+      <c r="C112" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="23" t="s">
+      <c r="A113" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="B113" s="24" t="s">
+      <c r="B113" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="C113" s="13" t="s">
+      <c r="C113" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="23" t="s">
+      <c r="A114" s="18" t="s">
         <v>341</v>
       </c>
-      <c r="B114" s="24" t="s">
+      <c r="B114" s="19" t="s">
         <v>334</v>
       </c>
-      <c r="C114" s="20" t="s">
+      <c r="C114" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="23" t="s">
+      <c r="A115" s="18" t="s">
         <v>332</v>
       </c>
-      <c r="B115" s="24" t="s">
+      <c r="B115" s="19" t="s">
         <v>346</v>
       </c>
-      <c r="C115" s="20" t="s">
+      <c r="C115" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="23" t="s">
+      <c r="A116" s="18" t="s">
         <v>338</v>
       </c>
-      <c r="B116" s="24" t="s">
+      <c r="B116" s="19" t="s">
         <v>334</v>
       </c>
-      <c r="C116" s="20" t="s">
+      <c r="C116" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="23" t="s">
+      <c r="A117" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="B117" s="24" t="s">
+      <c r="B117" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="C117" s="13" t="s">
+      <c r="C117" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="23" t="s">
+      <c r="A118" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="B118" s="24" t="s">
+      <c r="B118" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="C118" s="13" t="s">
+      <c r="C118" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="23" t="s">
+      <c r="A119" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="B119" s="24" t="s">
+      <c r="B119" s="19" t="s">
         <v>312</v>
       </c>
-      <c r="C119" s="20" t="s">
+      <c r="C119" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="23" t="s">
+      <c r="A120" s="18" t="s">
         <v>313</v>
       </c>
-      <c r="B120" s="24" t="s">
+      <c r="B120" s="19" t="s">
         <v>312</v>
       </c>
-      <c r="C120" s="20" t="s">
+      <c r="C120" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="23" t="s">
+      <c r="A121" s="18" t="s">
         <v>314</v>
       </c>
-      <c r="B121" s="24" t="s">
+      <c r="B121" s="19" t="s">
         <v>312</v>
       </c>
-      <c r="C121" s="20" t="s">
+      <c r="C121" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="23" t="s">
+      <c r="A122" s="18" t="s">
         <v>315</v>
       </c>
-      <c r="B122" s="24" t="s">
+      <c r="B122" s="19" t="s">
         <v>312</v>
       </c>
-      <c r="C122" s="20" t="s">
+      <c r="C122" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="23" t="s">
+      <c r="A123" s="18" t="s">
         <v>316</v>
       </c>
-      <c r="B123" s="24" t="s">
+      <c r="B123" s="19" t="s">
         <v>312</v>
       </c>
-      <c r="C123" s="20" t="s">
+      <c r="C123" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="23" t="s">
+      <c r="A124" s="18" t="s">
         <v>317</v>
       </c>
-      <c r="B124" s="24" t="s">
+      <c r="B124" s="19" t="s">
         <v>312</v>
       </c>
-      <c r="C124" s="20" t="s">
+      <c r="C124" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="23" t="s">
+      <c r="A125" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="B125" s="24" t="s">
+      <c r="B125" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="C125" s="13" t="s">
+      <c r="C125" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="23" t="s">
+      <c r="A126" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="B126" s="24" t="s">
+      <c r="B126" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="C126" s="13" t="s">
+      <c r="C126" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="23" t="s">
+      <c r="A127" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="B127" s="24" t="s">
+      <c r="B127" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="C127" s="13" t="s">
+      <c r="C127" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="23" t="s">
+      <c r="A128" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B128" s="24" t="s">
+      <c r="B128" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C128" s="13" t="s">
+      <c r="C128" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="23" t="s">
+      <c r="A129" s="18" t="s">
         <v>329</v>
       </c>
-      <c r="B129" s="24" t="s">
+      <c r="B129" s="19" t="s">
         <v>330</v>
       </c>
-      <c r="C129" s="20" t="s">
+      <c r="C129" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="23" t="s">
+      <c r="A130" s="18" t="s">
         <v>250</v>
       </c>
-      <c r="B130" s="24" t="s">
+      <c r="B130" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="C130" s="13" t="s">
+      <c r="C130" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="23" t="s">
+      <c r="A131" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B131" s="24" t="s">
+      <c r="B131" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C131" s="13" t="s">
+      <c r="C131" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="25" t="s">
+      <c r="A132" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="B132" s="26" t="s">
+      <c r="B132" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="C132" s="13" t="s">
+      <c r="C132" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="23" t="s">
+      <c r="A133" s="18" t="s">
         <v>267</v>
       </c>
-      <c r="B133" s="24" t="s">
+      <c r="B133" s="19" t="s">
         <v>268</v>
       </c>
-      <c r="C133" s="13" t="s">
+      <c r="C133" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="23" t="s">
+      <c r="A134" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="B134" s="24" t="s">
+      <c r="B134" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="C134" s="13" t="s">
+      <c r="C134" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" s="23" t="s">
+      <c r="A135" s="18" t="s">
         <v>325</v>
       </c>
-      <c r="B135" s="24" t="s">
+      <c r="B135" s="19" t="s">
         <v>326</v>
       </c>
-      <c r="C135" s="20" t="s">
+      <c r="C135" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" s="23" t="s">
+      <c r="A136" s="18" t="s">
         <v>287</v>
       </c>
-      <c r="B136" s="24" t="s">
+      <c r="B136" s="19" t="s">
         <v>288</v>
       </c>
-      <c r="C136" s="20" t="s">
+      <c r="C136" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" s="23" t="s">
+      <c r="A137" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="B137" s="24" t="s">
+      <c r="B137" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="C137" s="13" t="s">
+      <c r="C137" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="23" t="s">
+      <c r="A138" s="18" t="s">
         <v>342</v>
       </c>
-      <c r="B138" s="24" t="s">
+      <c r="B138" s="19" t="s">
         <v>334</v>
       </c>
-      <c r="C138" s="20" t="s">
+      <c r="C138" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" s="23" t="s">
+      <c r="A139" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="B139" s="24" t="s">
+      <c r="B139" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="C139" s="13" t="s">
+      <c r="C139" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" s="23" t="s">
+      <c r="A140" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="B140" s="24" t="s">
+      <c r="B140" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="C140" s="13" t="s">
+      <c r="C140" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" s="23" t="s">
+      <c r="A141" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="B141" s="24" t="s">
+      <c r="B141" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="C141" s="13" t="s">
+      <c r="C141" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" s="23" t="s">
+      <c r="A142" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="B142" s="24" t="s">
+      <c r="B142" s="19" t="s">
         <v>195</v>
       </c>
-      <c r="C142" s="13" t="s">
+      <c r="C142" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" s="23" t="s">
+      <c r="A143" s="18" t="s">
         <v>225</v>
       </c>
-      <c r="B143" s="24" t="s">
+      <c r="B143" s="19" t="s">
         <v>226</v>
       </c>
-      <c r="C143" s="13" t="s">
+      <c r="C143" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" s="23" t="s">
+      <c r="A144" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B144" s="24" t="s">
+      <c r="B144" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C144" s="13" t="s">
+      <c r="C144" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" s="23" t="s">
+      <c r="A145" s="18" t="s">
         <v>269</v>
       </c>
-      <c r="B145" s="24" t="s">
+      <c r="B145" s="19" t="s">
         <v>270</v>
       </c>
-      <c r="C145" s="13" t="s">
+      <c r="C145" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" s="23" t="s">
+      <c r="A146" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="B146" s="24" t="s">
+      <c r="B146" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="C146" s="13" t="s">
+      <c r="C146" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" s="23" t="s">
+      <c r="A147" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="B147" s="24" t="s">
+      <c r="B147" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="C147" s="13" t="s">
+      <c r="C147" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" s="23" t="s">
+      <c r="A148" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="B148" s="24" t="s">
+      <c r="B148" s="19" t="s">
         <v>228</v>
       </c>
-      <c r="C148" s="13" t="s">
+      <c r="C148" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" s="23" t="s">
+      <c r="A149" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B149" s="24" t="s">
+      <c r="B149" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C149" s="13" t="s">
+      <c r="C149" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A150" s="23" t="s">
+      <c r="A150" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="B150" s="24" t="s">
+      <c r="B150" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="C150" s="13" t="s">
+      <c r="C150" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151" s="23" t="s">
+      <c r="A151" s="18" t="s">
         <v>271</v>
       </c>
-      <c r="B151" s="24" t="s">
+      <c r="B151" s="19" t="s">
         <v>272</v>
       </c>
-      <c r="C151" s="13" t="s">
+      <c r="C151" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152" s="23" t="s">
+      <c r="A152" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="B152" s="24" t="s">
+      <c r="B152" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="C152" s="13" t="s">
+      <c r="C152" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153" s="23" t="s">
+      <c r="A153" s="18" t="s">
         <v>296</v>
       </c>
-      <c r="B153" s="24" t="s">
+      <c r="B153" s="19" t="s">
         <v>297</v>
       </c>
-      <c r="C153" s="20" t="s">
+      <c r="C153" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" s="23" t="s">
+      <c r="A154" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="B154" s="24" t="s">
+      <c r="B154" s="19" t="s">
         <v>300</v>
       </c>
-      <c r="C154" s="20" t="s">
+      <c r="C154" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" s="23" t="s">
+      <c r="A155" s="18" t="s">
         <v>298</v>
       </c>
-      <c r="B155" s="24" t="s">
+      <c r="B155" s="19" t="s">
         <v>297</v>
       </c>
-      <c r="C155" s="20" t="s">
+      <c r="C155" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156" s="23" t="s">
+      <c r="A156" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B156" s="24" t="s">
+      <c r="B156" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C156" s="13" t="s">
+      <c r="C156" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157" s="23" t="s">
+      <c r="A157" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="B157" s="24" t="s">
+      <c r="B157" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="C157" s="13" t="s">
+      <c r="C157" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A158" s="23" t="s">
+      <c r="A158" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="B158" s="24" t="s">
+      <c r="B158" s="19" t="s">
         <v>255</v>
       </c>
-      <c r="C158" s="13" t="s">
+      <c r="C158" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A159" s="23" t="s">
+      <c r="A159" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B159" s="24" t="s">
+      <c r="B159" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C159" s="13" t="s">
+      <c r="C159" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A160" s="23" t="s">
+      <c r="A160" s="18" t="s">
         <v>256</v>
       </c>
-      <c r="B160" s="24" t="s">
+      <c r="B160" s="19" t="s">
         <v>257</v>
       </c>
-      <c r="C160" s="13" t="s">
+      <c r="C160" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" s="23" t="s">
+      <c r="A161" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="B161" s="24" t="s">
+      <c r="B161" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="C161" s="13" t="s">
+      <c r="C161" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" s="23" t="s">
+      <c r="A162" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B162" s="24" t="s">
+      <c r="B162" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C162" s="13" t="s">
+      <c r="C162" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" s="23" t="s">
+      <c r="A163" s="18" t="s">
         <v>258</v>
       </c>
-      <c r="B163" s="24" t="s">
+      <c r="B163" s="19" t="s">
         <v>259</v>
       </c>
-      <c r="C163" s="13" t="s">
+      <c r="C163" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" s="23" t="s">
+      <c r="A164" s="18" t="s">
         <v>273</v>
       </c>
-      <c r="B164" s="24" t="s">
+      <c r="B164" s="19" t="s">
         <v>274</v>
       </c>
-      <c r="C164" s="13" t="s">
+      <c r="C164" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A165" s="23" t="s">
+      <c r="A165" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B165" s="24" t="s">
+      <c r="B165" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C165" s="13" t="s">
+      <c r="C165" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A166" s="23" t="s">
+      <c r="A166" s="18" t="s">
         <v>305</v>
       </c>
-      <c r="B166" s="24" t="s">
+      <c r="B166" s="19" t="s">
         <v>306</v>
       </c>
-      <c r="C166" s="20" t="s">
+      <c r="C166" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" s="23" t="s">
+      <c r="A167" s="18" t="s">
         <v>308</v>
       </c>
-      <c r="B167" s="24" t="s">
+      <c r="B167" s="19" t="s">
         <v>309</v>
       </c>
-      <c r="C167" s="20" t="s">
+      <c r="C167" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" s="23" t="s">
+      <c r="A168" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="B168" s="24" t="s">
+      <c r="B168" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="C168" s="13" t="s">
+      <c r="C168" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A169" s="23" t="s">
+      <c r="A169" s="18" t="s">
         <v>307</v>
       </c>
-      <c r="B169" s="24" t="s">
+      <c r="B169" s="19" t="s">
         <v>306</v>
       </c>
-      <c r="C169" s="20" t="s">
+      <c r="C169" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A170" s="23" t="s">
+      <c r="A170" s="18" t="s">
         <v>310</v>
       </c>
-      <c r="B170" s="24" t="s">
+      <c r="B170" s="19" t="s">
         <v>309</v>
       </c>
-      <c r="C170" s="20" t="s">
+      <c r="C170" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A171" s="23" t="s">
+      <c r="A171" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="B171" s="24" t="s">
+      <c r="B171" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="C171" s="13" t="s">
+      <c r="C171" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" s="23" t="s">
+      <c r="A172" s="18" t="s">
         <v>337</v>
       </c>
-      <c r="B172" s="24" t="s">
+      <c r="B172" s="19" t="s">
         <v>334</v>
       </c>
-      <c r="C172" s="20" t="s">
+      <c r="C172" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A173" s="23" t="s">
+      <c r="A173" s="18" t="s">
         <v>331</v>
       </c>
-      <c r="B173" s="24" t="s">
+      <c r="B173" s="19" t="s">
         <v>347</v>
       </c>
-      <c r="C173" s="20" t="s">
+      <c r="C173" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A174" s="23" t="s">
+      <c r="A174" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="B174" s="24" t="s">
+      <c r="B174" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="C174" s="13" t="s">
+      <c r="C174" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" s="23" t="s">
+      <c r="A175" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="B175" s="24" t="s">
+      <c r="B175" s="19" t="s">
         <v>203</v>
       </c>
-      <c r="C175" s="13" t="s">
+      <c r="C175" s="10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A176" s="23" t="s">
+      <c r="A176" s="18" t="s">
         <v>336</v>
       </c>
-      <c r="B176" s="24" t="s">
+      <c r="B176" s="19" t="s">
         <v>334</v>
       </c>
-      <c r="C176" s="20" t="s">
+      <c r="C176" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" s="23" t="s">
+      <c r="A177" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="B177" s="24" t="s">
+      <c r="B177" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="C177" s="13" t="s">
+      <c r="C177" s="10" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A178" s="23" t="s">
+      <c r="A178" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B178" s="24" t="s">
+      <c r="B178" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C178" s="13" t="s">
+      <c r="C178" s="10" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A179" s="25" t="s">
+      <c r="A179" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="B179" s="26" t="s">
+      <c r="B179" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C179" s="27" t="s">
+      <c r="C179" s="22" t="s">
         <v>279</v>
       </c>
     </row>
@@ -5818,18 +6418,6 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80036CEE-20A2-4D5B-894A-BFFA26FC4F58}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>